<commit_message>
auto envio de horarios
</commit_message>
<xml_diff>
--- a/InscripcionEncuestasSemana1/Formulario inscripción a charlas vocacionales (Respuestas).xlsx
+++ b/InscripcionEncuestasSemana1/Formulario inscripción a charlas vocacionales (Respuestas).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="94">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Instrucción de yoga - Miércoles 29 de Septiembre de 15 a 16 hrs. </t>
   </si>
   <si>
-    <t>Jefa servicio a bordo LATAM Chile - Miércoles 29 de Septiembre de 15 a 16 hrs. (¡mismo horario de la charla anterior!)</t>
+    <t>Servicio a Bordo Aerolínea - Miércoles 29 de Septiembre de 15 a 16 hrs. (¡mismo horario de la charla anterior!)</t>
   </si>
   <si>
     <t xml:space="preserve">Sociedad civil - Miércoles 29 de Septiembre de 16 a 17 hrs. </t>
@@ -197,6 +197,102 @@
   </si>
   <si>
     <t>ivalencia@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>awiele@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>msubiabre@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>mtorres@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>egallardo@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>jllano@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>vprades1@gmail.com</t>
+  </si>
+  <si>
+    <t>mcrignola@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>lprado@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>blara@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>vpiffardi@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>salegria@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>federicopereirazz@gmail.com</t>
+  </si>
+  <si>
+    <t>jcortes@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>slanger@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>andreacweger@gmail.com</t>
+  </si>
+  <si>
+    <t>aaliaga@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>mrapp@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>simoya@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>ekosche@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>arocco@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>jklesse@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>jkohan@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>sjorquera@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>Mprades@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>ebernal@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>dmachuca@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>candrade@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>brojas@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>cfrei@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>cmontes@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>ctorres@dsmorus.cl</t>
+  </si>
+  <si>
+    <t>fordenes@dsmorus.cl</t>
   </si>
 </sst>
 </file>
@@ -206,7 +302,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -216,6 +312,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,11 +328,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -498,7 +598,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -527,677 +627,1205 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>44463.591557175925</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>44463.59252446759</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>44463.59262574074</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>44463.593432407404</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>44463.597352916666</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T6" s="3" t="s">
+      <c r="H6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>44463.59811449074</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="3" t="s">
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>44463.59904725694</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="3" t="s">
+      <c r="K8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>44463.59940041667</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T9" s="3" t="s">
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>44463.59992976852</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T10" s="3" t="s">
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>44463.602713333334</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>44463.609010416665</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>44463.61065173611</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>44463.620988877316</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O14" s="3" t="s">
+      <c r="E14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>44463.631718449076</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>44463.66222384259</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O16" s="3" t="s">
+      <c r="E16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>44463.673006516205</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T17" s="3" t="s">
+      <c r="J17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>44463.67370829861</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N18" s="3" t="s">
+      <c r="I18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>44463.677787650464</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>44463.68508981481</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P20" s="3" t="s">
+      <c r="I20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>44463.69589001157</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P21" s="3" t="s">
+      <c r="D21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <v>44463.70910021991</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2">
+      <c r="A23" s="3">
         <v>44463.712641018516</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="3" t="s">
+      <c r="D23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <v>44463.753718402775</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O24" s="3" t="s">
+      <c r="E24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <v>44463.762655115745</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L25" s="3" t="s">
+      <c r="D25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2">
+      <c r="A26" s="3">
         <v>44463.799716180554</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P26" s="3" t="s">
+      <c r="H26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P26" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2">
+      <c r="A27" s="3">
         <v>44463.80786731481</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2">
+      <c r="A28" s="3">
         <v>44463.80843828704</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R28" s="3" t="s">
+      <c r="D28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R28" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2">
+      <c r="A29" s="3">
         <v>44463.82647717593</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T29" s="3" t="s">
+      <c r="I29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T29" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
         <v>44463.82786208333</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="S30" s="3" t="s">
+      <c r="S30" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2">
+      <c r="A31" s="3">
         <v>44463.85876846065</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T31" s="3" t="s">
+      <c r="C31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T31" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2">
+      <c r="A32" s="3">
         <v>44463.951220567134</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N32" s="3" t="s">
+      <c r="I32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N32" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2">
+      <c r="A33" s="3">
         <v>44464.47845767361</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="N33" s="3" t="s">
+      <c r="N33" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2">
+      <c r="A34" s="3">
         <v>44464.62160358796</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2">
+      <c r="A35" s="3">
         <v>44464.62905510417</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T35" s="3" t="s">
+      <c r="F35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T35" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2">
+      <c r="A36" s="3">
         <v>44464.64547315972</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T36" s="3" t="s">
+      <c r="G36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T36" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2">
+      <c r="A37" s="3">
         <v>44464.67903641204</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O37" s="3" t="s">
+      <c r="O37" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2">
+      <c r="A38" s="3">
         <v>44464.69703285879</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38" s="3" t="s">
+      <c r="E38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2">
+      <c r="A39" s="3">
         <v>44464.69759481482</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2">
+      <c r="A40" s="3">
         <v>44464.69906450232</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S40" s="3" t="s">
+      <c r="C40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S40" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2">
+      <c r="A41" s="3">
         <v>44464.77032144676</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N41" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R41" s="3" t="s">
+      <c r="D41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R41" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2">
+      <c r="A42" s="3">
         <v>44464.806304791666</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T42" s="3" t="s">
+      <c r="F42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T42" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2">
+      <c r="A43" s="3">
         <v>44465.50636681713</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T43" s="3" t="s">
+      <c r="I43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T43" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3">
+        <v>44465.5310790625</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3">
+        <v>44465.53555302083</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3">
+        <v>44465.53808550926</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3">
+        <v>44465.5392989699</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3">
+        <v>44465.56849447917</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3">
+        <v>44465.6191680787</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S49" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3">
+        <v>44465.62611869213</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T50" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3">
+        <v>44465.87583310185</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3">
+        <v>44465.89283024306</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S52" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3">
+        <v>44465.955002511575</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3">
+        <v>44465.99205144676</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T54" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3">
+        <v>44466.342979884255</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O55" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3">
+        <v>44466.369900578706</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P56" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3">
+        <v>44466.45729268518</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3">
+        <v>44466.46377689815</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3">
+        <v>44466.46609403935</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O59" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3">
+        <v>44466.49036489583</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O60" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3">
+        <v>44466.52045956018</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O61" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P61" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3">
+        <v>44466.56686096065</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3">
+        <v>44466.56692935185</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="3">
+        <v>44466.56948978009</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P64" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="3">
+        <v>44466.56983429399</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3">
+        <v>44466.624182685184</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="3">
+        <v>44466.6264496875</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3">
+        <v>44466.62881501157</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P68" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="3">
+        <v>44466.62899394676</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3">
+        <v>44466.63244527778</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3">
+        <v>44466.637521365745</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T71" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3">
+        <v>44466.65736049769</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="T72" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3">
+        <v>44466.67227461806</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N73" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O73" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3">
+        <v>44466.6772240162</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N74" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3">
+        <v>44466.6856837963</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N75" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O75" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q75" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3">
+        <v>44466.69628685185</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N76" s="4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>